<commit_message>
fuck my life again
</commit_message>
<xml_diff>
--- a/PTTK HTTT/Project/BangPhanCong.xlsx
+++ b/PTTK HTTT/Project/BangPhanCong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/183e42ef57ca74cb/Desktop/SGU-Course/PTTK HTTT/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{BDDD7547-96DB-417B-BED7-148E08AAD1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43399253-BD45-4D4A-970F-94F7753D1E8A}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{BDDD7547-96DB-417B-BED7-148E08AAD1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{544E3151-DC2C-49A1-AD7B-9CE58ADA0003}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="14374" xr2:uid="{BDA39A5F-4239-4D48-B4A2-DDF09E00B8C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{BDA39A5F-4239-4D48-B4A2-DDF09E00B8C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Công việc</t>
   </si>
@@ -73,22 +73,22 @@
     <t>Lộc, Thiện, Minh, Huy</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>Tuần 6-8</t>
   </si>
   <si>
     <t>Tuần 8-11</t>
   </si>
   <si>
-    <t>Nhóm: 8  _ STT:</t>
-  </si>
-  <si>
     <t>Bảng lập kế hoạch</t>
   </si>
   <si>
     <t>Tuần 12-14</t>
+  </si>
+  <si>
+    <t>Nhóm: 8</t>
+  </si>
+  <si>
+    <t>STT: 9</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -203,11 +203,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -226,6 +252,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,15 +261,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -558,55 +577,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FDB2CFD-14DD-4853-B610-D15BD0C53E40}">
-  <dimension ref="F4:P17"/>
+  <dimension ref="F1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.3" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="18.109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="6:16" ht="22.25" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="6:13" ht="22.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="6:16" ht="22.25" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="6:13" ht="22.2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
+      <c r="H5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="6:16" ht="22.25" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="6:13" ht="22.2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -616,7 +641,7 @@
       <c r="L7" s="4"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="5" t="s">
@@ -631,11 +656,8 @@
       <c r="K8" s="3"/>
       <c r="L8" s="4"/>
       <c r="M8" s="2"/>
-      <c r="P8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
       <c r="H9" s="6" t="s">
@@ -649,9 +671,8 @@
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>
       <c r="H10" s="6" t="s">
@@ -666,18 +687,15 @@
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
       <c r="H11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>11</v>
@@ -686,14 +704,14 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="12" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
       <c r="H12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J12" s="7" t="s">
         <v>11</v>
@@ -702,14 +720,14 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F13" s="2"/>
       <c r="G13" s="3"/>
       <c r="H13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>11</v>
@@ -718,7 +736,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -728,7 +746,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="15" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -738,7 +756,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="6:16" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -748,7 +766,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="6:13" ht="21.6" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:13" ht="21.6" x14ac:dyDescent="0.4">
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -759,8 +777,7 @@
       <c r="M17" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="H5:J5"/>
+  <mergeCells count="1">
     <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>